<commit_message>
started with api, fixed problem with nonsense mutations, corrected manually some of those mutations, fixed bug when checking errors in manually corrected if the name of the allele had been changed (commented line in format_manual_changes)
</commit_message>
<xml_diff>
--- a/manual_fixes_pombase/allele_cannot_fix.xlsx
+++ b/manual_fixes_pombase/allele_cannot_fix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manu/Documents/Projects/allele_qc/manual_fixes_pombase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53BE93C-E461-EA4A-A3F0-309624547474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{346D4458-EE12-B24D-AEEA-CC5E984CDB1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" xr2:uid="{1CD96D0D-EF95-4347-8CEF-0F0E0E511B79}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14420" activeTab="1" xr2:uid="{1CD96D0D-EF95-4347-8CEF-0F0E0E511B79}"/>
   </bookViews>
   <sheets>
     <sheet name="identified" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4935" uniqueCount="2566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4968" uniqueCount="2592">
   <si>
     <t>systematic_id</t>
   </si>
@@ -7763,13 +7763,91 @@
   </si>
   <si>
     <t>sequence_error</t>
+  </si>
+  <si>
+    <t>rad23-1</t>
+  </si>
+  <si>
+    <t>Q232*</t>
+  </si>
+  <si>
+    <t>sre1-Q801*</t>
+  </si>
+  <si>
+    <t>sre1-Q802*</t>
+  </si>
+  <si>
+    <t>Q802*</t>
+  </si>
+  <si>
+    <t>dsc2-G160*</t>
+  </si>
+  <si>
+    <t>elf1-21</t>
+  </si>
+  <si>
+    <t>ssu72-1-86</t>
+  </si>
+  <si>
+    <t>spo3m (KC51)</t>
+  </si>
+  <si>
+    <t>pst1-1</t>
+  </si>
+  <si>
+    <t>lcf1-W376-&gt;stop</t>
+  </si>
+  <si>
+    <t>pdf1-K302Stop</t>
+  </si>
+  <si>
+    <t>dot2-439</t>
+  </si>
+  <si>
+    <t>atg7-m1</t>
+  </si>
+  <si>
+    <t>V160*</t>
+  </si>
+  <si>
+    <t>dsc2-V160*</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Q863*</t>
+  </si>
+  <si>
+    <t>W427*</t>
+  </si>
+  <si>
+    <t>W1305*</t>
+  </si>
+  <si>
+    <t>W367*</t>
+  </si>
+  <si>
+    <t>probably typo in paper</t>
+  </si>
+  <si>
+    <t>K321*</t>
+  </si>
+  <si>
+    <t>E33*</t>
+  </si>
+  <si>
+    <t>typo in main text of paper, correct in figure legend and image</t>
+  </si>
+  <si>
+    <t>W227*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -7873,6 +7951,12 @@
       <name val="Menlo"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -7960,7 +8044,7 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -8010,6 +8094,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="40% - Accent1" xfId="5" builtinId="31"/>
@@ -8337,8 +8422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29D01E91-6EC0-A840-8F42-8EB098335027}">
   <dimension ref="A1:V456"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28903,10 +28988,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F3C769F-4A95-764B-9459-4A83F92E8C6E}">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28914,10 +28999,11 @@
     <col min="1" max="1" width="16.5" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="81.33203125" style="7" customWidth="1"/>
     <col min="3" max="3" width="27.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="7"/>
+    <col min="4" max="4" width="55.5" style="7" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -28927,8 +29013,14 @@
       <c r="C1" s="7" t="s">
         <v>2289</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="7" t="s">
+        <v>2282</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>2582</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>2259</v>
       </c>
@@ -28936,7 +29028,7 @@
         <v>2260</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>2297</v>
       </c>
@@ -28944,7 +29036,7 @@
         <v>2299</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>2298</v>
       </c>
@@ -28952,7 +29044,7 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>2310</v>
       </c>
@@ -28960,7 +29052,7 @@
         <v>2309</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>2323</v>
       </c>
@@ -28968,7 +29060,7 @@
         <v>2325</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>2324</v>
       </c>
@@ -28976,7 +29068,7 @@
         <v>2326</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>2333</v>
       </c>
@@ -28984,7 +29076,7 @@
         <v>2336</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>2334</v>
       </c>
@@ -28992,7 +29084,7 @@
         <v>2337</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>2335</v>
       </c>
@@ -29000,7 +29092,7 @@
         <v>2338</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>2384</v>
       </c>
@@ -29008,7 +29100,7 @@
         <v>2385</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>2388</v>
       </c>
@@ -29016,7 +29108,7 @@
         <v>2529</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>2400</v>
       </c>
@@ -29024,7 +29116,7 @@
         <v>2415</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>2401</v>
       </c>
@@ -29032,7 +29124,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>2402</v>
       </c>
@@ -29040,7 +29132,7 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>2403</v>
       </c>
@@ -29184,7 +29276,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
         <v>2510</v>
       </c>
@@ -29192,7 +29284,7 @@
         <v>2512</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>2513</v>
       </c>
@@ -29201,6 +29293,121 @@
       </c>
       <c r="C34" s="7" t="s">
         <v>108</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="s">
+        <v>2566</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>2567</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="7" t="s">
+        <v>2568</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>2570</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>2569</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="47" t="s">
+        <v>2571</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>2580</v>
+      </c>
+      <c r="D37" s="47" t="s">
+        <v>2581</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>2456</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="47" t="s">
+        <v>2572</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>2583</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>2456</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="47" t="s">
+        <v>2573</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>2352</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="47" t="s">
+        <v>2574</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>2584</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>2456</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="47" t="s">
+        <v>2575</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>2585</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>2456</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="47" t="s">
+        <v>2576</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>2586</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>2587</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="47" t="s">
+        <v>2577</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>2588</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="47" t="s">
+        <v>2578</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>2589</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>2590</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="47" t="s">
+        <v>2579</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>2591</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>2456</v>
       </c>
     </row>
   </sheetData>

</xml_diff>